<commit_message>
tweaks to ontology data
</commit_message>
<xml_diff>
--- a/data/tjbrailey_psp_ontology.xlsx
+++ b/data/tjbrailey_psp_ontology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbrai\Dropbox\github_private\SeniorThesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F850A8-D0B0-4946-9A11-9AFCD8EB4A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F9E200-7571-4E05-A227-FEE6C4C7965B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{5F6FE1F0-E09E-4F56-AA05-9EA20A06C7BA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{5F6FE1F0-E09E-4F56-AA05-9EA20A06C7BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="128">
   <si>
     <t>child_0</t>
   </si>
@@ -467,6 +467,18 @@
   </si>
   <si>
     <t>vertical power-sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ethnofederalism </t>
+  </si>
+  <si>
+    <t>Roeder, Philip G. (2009).</t>
+  </si>
+  <si>
+    <t>ethnofederalism</t>
+  </si>
+  <si>
+    <t>Roeder, Philip G. 2009. ‘Ethnofederalism and the Mismanagement of Conflicting Nationalisms’. Regional &amp; Federal Studies 19(2): 203–19.</t>
   </si>
 </sst>
 </file>
@@ -547,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -566,6 +578,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,9 +895,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DD2C77-0DD6-4042-9A1C-B14AA519E332}">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
@@ -2445,6 +2462,23 @@
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
     </row>
+    <row r="81" spans="1:4" ht="64" x14ac:dyDescent="0.5">
+      <c r="A81" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="D82" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2453,10 +2487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B9ED45C-9EA4-41A1-9D1E-2F0E66E277EF}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2483,22 +2517,21 @@
         <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="5"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -2506,11 +2539,11 @@
       <c r="A4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>115</v>
+      <c r="B4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -2519,10 +2552,10 @@
         <v>74</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -2531,10 +2564,10 @@
         <v>74</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -2543,10 +2576,10 @@
         <v>74</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -2555,23 +2588,29 @@
         <v>74</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
@@ -2626,7 +2665,7 @@
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="2"/>
@@ -2656,7 +2695,7 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" s="2"/>
@@ -2740,7 +2779,7 @@
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="7"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A40" s="2"/>
@@ -2860,7 +2899,7 @@
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A60" s="2"/>
@@ -2872,7 +2911,7 @@
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="5"/>
-      <c r="D61" s="6"/>
+      <c r="D61" s="5"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A62" s="2"/>
@@ -2896,7 +2935,7 @@
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A66" s="2"/>
@@ -2988,52 +3027,58 @@
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C81" s="8"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.5">
       <c r="C82" s="8"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.5">
       <c r="C83" s="8"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.5">
       <c r="C84" s="8"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A85" s="3"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="5"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="C85" s="8"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A86" s="3"/>
       <c r="B86" s="2"/>
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A87" s="3"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B87" s="2"/>
+      <c r="C87" s="5"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A88" s="3"/>
       <c r="B88" s="7"/>
-      <c r="C88" s="5"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C88" s="7"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A89" s="3"/>
       <c r="B89" s="7"/>
-      <c r="C89" s="6"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C89" s="5"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A90" s="3"/>
       <c r="B90" s="7"/>
       <c r="C90" s="6"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A91" s="3"/>
       <c r="B91" s="7"/>
-      <c r="C91" s="5"/>
+      <c r="C91" s="6"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A92" s="3"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>